<commit_message>
Leaf traits + suppl. figure
</commit_message>
<xml_diff>
--- a/DATA/Spatial_Campaign_data.xlsx
+++ b/DATA/Spatial_Campaign_data.xlsx
@@ -1043,6 +1043,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1342,9 +1346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K117" sqref="K117"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>